<commit_message>
add VPC figures (#12)
</commit_message>
<xml_diff>
--- a/test/test_NO1/prepareInput/Workflow.xlsx
+++ b/test/test_NO1/prepareInput/Workflow.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="408" windowWidth="19464" windowHeight="7680" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="408" windowWidth="19464" windowHeight="7680"/>
   </bookViews>
   <sheets>
     <sheet name="Workflow" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="128">
   <si>
     <t>Code Identifier</t>
   </si>
@@ -390,6 +390,21 @@
   </si>
   <si>
     <t>Output 5</t>
+  </si>
+  <si>
+    <t>Sensitivity</t>
+  </si>
+  <si>
+    <t>sensXls</t>
+  </si>
+  <si>
+    <t>xlsfilefor sensitivity Parameter definition; if it is empty, sheet is in this xlsfile</t>
+  </si>
+  <si>
+    <t>sensSheet</t>
+  </si>
+  <si>
+    <t>xlssheet for sensitivity Parameter definition; if empty first sheet is taken</t>
   </si>
 </sst>
 </file>
@@ -825,10 +840,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F26"/>
+  <dimension ref="A1:F29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1069,63 +1084,53 @@
       </c>
     </row>
     <row r="22" spans="1:6" ht="49.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="10"/>
-      <c r="B22" s="11" t="s">
-        <v>45</v>
-      </c>
-      <c r="C22" s="10"/>
+      <c r="A22" s="7"/>
+      <c r="B22" s="8" t="s">
+        <v>123</v>
+      </c>
+      <c r="C22" s="7"/>
       <c r="D22" s="7"/>
       <c r="E22" s="7"/>
       <c r="F22" s="7"/>
     </row>
     <row r="23" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A23" s="9" t="s">
-        <v>46</v>
+        <v>124</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="C23">
-        <v>1</v>
+        <v>125</v>
       </c>
       <c r="D23" s="7"/>
       <c r="E23" s="7"/>
       <c r="F23" s="7"/>
     </row>
-    <row r="24" spans="1:6" ht="39.6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A24" s="9" t="s">
-        <v>48</v>
+        <v>126</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="C24">
-        <v>1</v>
+        <v>127</v>
       </c>
       <c r="D24" s="7"/>
       <c r="E24" s="7"/>
       <c r="F24" s="7"/>
     </row>
     <row r="25" spans="1:6" ht="13.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="B25" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="C25">
-        <v>1</v>
-      </c>
+      <c r="A25" s="10"/>
+      <c r="B25" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="C25" s="10"/>
       <c r="D25" s="7"/>
       <c r="E25" s="7"/>
       <c r="F25" s="7"/>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A26" s="9" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="C26">
         <v>1</v>
@@ -1133,6 +1138,45 @@
       <c r="D26" s="7"/>
       <c r="E26" s="7"/>
       <c r="F26" s="7"/>
+    </row>
+    <row r="27" spans="1:6" ht="39.6" x14ac:dyDescent="0.25">
+      <c r="A27" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="C27">
+        <v>1</v>
+      </c>
+      <c r="D27" s="7"/>
+      <c r="E27" s="7"/>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C28">
+        <v>0</v>
+      </c>
+      <c r="D28" s="7"/>
+      <c r="E28" s="7"/>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="C29">
+        <v>0</v>
+      </c>
+      <c r="D29" s="7"/>
+      <c r="E29" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
@@ -1144,7 +1188,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I28" sqref="I28"/>
     </sheetView>
   </sheetViews>

</xml_diff>